<commit_message>
Updated Code to Detect NGO
</commit_message>
<xml_diff>
--- a/NGO LIST.xlsx
+++ b/NGO LIST.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Delete it\Yukti\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Pahal Jan Sahyog Vikas Sansthan</t>
   </si>
@@ -164,19 +169,16 @@
   </si>
   <si>
     <t>Cuddles Foundation</t>
+  </si>
+  <si>
+    <t>Health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,152 +198,8 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,194 +212,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -549,251 +221,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -808,68 +238,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -891,7 +277,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -933,7 +319,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -975,7 +361,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1017,7 +403,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1059,7 +445,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1101,7 +487,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1143,7 +529,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1185,7 +571,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1227,7 +613,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1269,7 +655,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1311,7 +697,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1353,7 +739,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1395,7 +781,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1437,7 +823,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1479,7 +865,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1521,7 +907,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1563,7 +949,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1605,7 +991,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1647,7 +1033,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1689,7 +1075,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1731,7 +1117,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1773,7 +1159,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1815,7 +1201,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1857,7 +1243,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1899,7 +1285,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1941,7 +1327,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1983,7 +1369,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2025,7 +1411,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2067,7 +1453,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2109,7 +1495,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2151,7 +1537,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2193,7 +1579,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2235,7 +1621,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2277,7 +1663,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2553,26 +1939,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="46.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="40.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="115.8" customHeight="1" spans="1:3">
+    <row r="1" spans="1:3" ht="115.8" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +1974,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="60" customHeight="1" spans="1:3">
+    <row r="3" spans="1:3" ht="60" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2604,7 +1990,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" ht="60" customHeight="1" spans="1:3">
+    <row r="5" spans="1:3" ht="60" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2620,7 +2006,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" ht="153" customHeight="1" spans="1:3">
+    <row r="7" spans="1:3" ht="153" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2636,7 +2022,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" ht="97.2" customHeight="1" spans="1:3">
+    <row r="9" spans="1:3" ht="97.2" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2652,7 +2038,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" ht="190.2" customHeight="1" spans="1:3">
+    <row r="11" spans="1:3" ht="190.2" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2668,7 +2054,7 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" ht="41.4" customHeight="1" spans="1:3">
+    <row r="13" spans="1:3" ht="41.4" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2684,7 +2070,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" ht="60" customHeight="1" spans="1:3">
+    <row r="15" spans="1:3" ht="60" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2700,7 +2086,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" ht="41.4" customHeight="1" spans="1:3">
+    <row r="17" spans="1:3" ht="41.4" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2716,12 +2102,12 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" ht="115.8" customHeight="1" spans="1:3">
+    <row r="19" spans="1:3" ht="115.8" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
@@ -2732,7 +2118,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" ht="97.2" customHeight="1" spans="1:3">
+    <row r="21" spans="1:3" ht="97.2" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2748,7 +2134,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" ht="97.2" customHeight="1" spans="1:3">
+    <row r="23" spans="1:3" ht="97.2" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2764,7 +2150,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" ht="115.8" customHeight="1" spans="1:3">
+    <row r="25" spans="1:3" ht="115.8" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2780,7 +2166,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" ht="78.6" customHeight="1" spans="1:3">
+    <row r="27" spans="1:3" ht="78.599999999999994" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2796,7 +2182,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" ht="78.6" customHeight="1" spans="1:3">
+    <row r="29" spans="1:3" ht="78.599999999999994" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -2812,7 +2198,7 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" ht="153" customHeight="1" spans="1:3">
+    <row r="31" spans="1:3" ht="153" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -2828,7 +2214,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" ht="190.2" customHeight="1" spans="1:3">
+    <row r="33" spans="1:3" ht="190.2" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -2844,7 +2230,7 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" ht="97.2" customHeight="1" spans="1:3">
+    <row r="35" spans="1:3" ht="97.2" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -2860,7 +2246,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" ht="246" customHeight="1" spans="1:3">
+    <row r="37" spans="1:3" ht="246" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -2876,7 +2262,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" ht="41.4" customHeight="1" spans="1:3">
+    <row r="39" spans="1:3" ht="41.4" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -2892,7 +2278,7 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" ht="97.2" customHeight="1" spans="1:3">
+    <row r="41" spans="1:3" ht="97.2" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -2908,7 +2294,7 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" ht="60" customHeight="1" spans="1:3">
+    <row r="43" spans="1:3" ht="60" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
@@ -2924,7 +2310,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" ht="97.2" customHeight="1" spans="1:3">
+    <row r="45" spans="1:3" ht="97.2" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
@@ -2940,7 +2326,7 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" ht="60" customHeight="1" spans="1:3">
+    <row r="47" spans="1:3" ht="60" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
@@ -2956,7 +2342,7 @@
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" ht="41.4" customHeight="1" spans="1:3">
+    <row r="49" spans="1:3" ht="41.4" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
@@ -2972,7 +2358,7 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" ht="78.6" customHeight="1" spans="1:3">
+    <row r="51" spans="1:3" ht="78.599999999999994" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
@@ -2988,7 +2374,7 @@
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" ht="60" customHeight="1" spans="1:3">
+    <row r="53" spans="1:3" ht="60" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
@@ -3004,7 +2390,7 @@
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" ht="134.4" customHeight="1" spans="1:3">
+    <row r="55" spans="1:3" ht="134.4" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -3020,7 +2406,7 @@
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" ht="283.2" customHeight="1" spans="1:3">
+    <row r="57" spans="1:3" ht="283.2" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>42</v>
       </c>
@@ -3036,7 +2422,7 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" ht="41.4" customHeight="1" spans="1:3">
+    <row r="59" spans="1:3" ht="41.4" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>43</v>
       </c>
@@ -3052,7 +2438,7 @@
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" ht="22.8" customHeight="1" spans="1:3">
+    <row r="61" spans="1:3" ht="22.8" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>44</v>
       </c>
@@ -3068,7 +2454,7 @@
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" ht="153" customHeight="1" spans="1:3">
+    <row r="63" spans="1:3" ht="153" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>46</v>
       </c>
@@ -3084,7 +2470,7 @@
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" ht="134.4" customHeight="1" spans="1:3">
+    <row r="65" spans="1:3" ht="134.4" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>48</v>
       </c>
@@ -3100,7 +2486,7 @@
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" ht="60" customHeight="1" spans="1:3">
+    <row r="67" spans="1:3" ht="60" customHeight="1">
       <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
@@ -3118,33 +2504,57 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="A57:A58"/>
     <mergeCell ref="A59:A60"/>
@@ -3169,60 +2579,35 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>